<commit_message>
edited the test cases doc
</commit_message>
<xml_diff>
--- a/DBA(Digital barrier analysis)/Additional features/Test cases DBA Additional features.xlsx
+++ b/DBA(Digital barrier analysis)/Additional features/Test cases DBA Additional features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Global settings page" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="198">
   <si>
     <t>S.N</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Validate that the UI of the global setting page is as per the design</t>
-  </si>
-  <si>
-    <t>The Ui of the global settings page should be as specified in the design.</t>
   </si>
   <si>
     <t>Preconditions:
@@ -463,9 +460,6 @@
     <t>The selected consequence type should be deleted from the list.</t>
   </si>
   <si>
-    <t>DBA_GlobalSettings_</t>
-  </si>
-  <si>
     <t>DBA_ExportRecords_UI</t>
   </si>
   <si>
@@ -474,6 +468,156 @@
   <si>
     <t xml:space="preserve">Preconditions:
 1. </t>
+  </si>
+  <si>
+    <t>The UI of the global settings page should be as specified in the design.</t>
+  </si>
+  <si>
+    <t>DBA_GlobalSettings_EditRiskMatrix</t>
+  </si>
+  <si>
+    <t>Vaidate that the risk matrix can be edited</t>
+  </si>
+  <si>
+    <t>Select the language in which you want to edit the risk matrix</t>
+  </si>
+  <si>
+    <t>The user should be able to edit the risk matrix in the selected language.</t>
+  </si>
+  <si>
+    <t>The loaded risk matrix should be in the selected language. The Probability and Consequence type of the risk matrix should be in the selected language.</t>
+  </si>
+  <si>
+    <t>Click on the edit button of the risk matrix table.</t>
+  </si>
+  <si>
+    <t>The "Save" button should appear and the name of the consequence and the probability should be editable. The color in each box of the table should also be editable.</t>
+  </si>
+  <si>
+    <t>Change the name of the consequences and probability.</t>
+  </si>
+  <si>
+    <t>Change the color of some cell.</t>
+  </si>
+  <si>
+    <t>The probability and consequence field should be editable</t>
+  </si>
+  <si>
+    <t>The color of the cells should be editable.</t>
+  </si>
+  <si>
+    <t>Click on "Save" button.</t>
+  </si>
+  <si>
+    <t>The Changes made should be saved and should be displayed in all the new projects created of the selected language.</t>
+  </si>
+  <si>
+    <t>DBA_GlobalSettings_AddDuplicateWorkType</t>
+  </si>
+  <si>
+    <t>Validate that work type with same name cannot be created.</t>
+  </si>
+  <si>
+    <t>The name of the Work Type should be unique.</t>
+  </si>
+  <si>
+    <t>Select the Language in which you want to add a Work Type(Suppose norwegian)</t>
+  </si>
+  <si>
+    <t>Create the work type with name "Test"(can be any name of your choice)</t>
+  </si>
+  <si>
+    <t>The Created Work Type should be added in the Work Type list with a success message.</t>
+  </si>
+  <si>
+    <t>Again create a work type with name "test".</t>
+  </si>
+  <si>
+    <t>The work type should not be created and the message "Duplicate Work Type" should be displayed.</t>
+  </si>
+  <si>
+    <t>DBA_GlobalSettings_AddDuplicateWorkOperation</t>
+  </si>
+  <si>
+    <t>The name of the Work operation under the selected work type should be unique.</t>
+  </si>
+  <si>
+    <t>Create the work operation with name "Test"(can be any name of your choice) under the selected WT</t>
+  </si>
+  <si>
+    <t>The Created Work Operation should be added in the Work Operation list with a success message under the selected wt.</t>
+  </si>
+  <si>
+    <t>Again create a work operation with name "test" under the same work type.</t>
+  </si>
+  <si>
+    <t>The work operation should not be created and the message "Duplicate Work operation should be displayed.</t>
+  </si>
+  <si>
+    <t>DBA_GlobalSettings_AddDuplicatePotentialIncident</t>
+  </si>
+  <si>
+    <t>Vlaidate that work operation with same name cannot be created under the same work type.</t>
+  </si>
+  <si>
+    <t>Validate that potential incident with the same name cannot be created under the same work type and work operation</t>
+  </si>
+  <si>
+    <t>The name of the potential incident under the selected work type and work operation should be unique.</t>
+  </si>
+  <si>
+    <t>Select the Language in which you want to add a Work Operation(Suppose norwegian)</t>
+  </si>
+  <si>
+    <t>Select the Language in which you want to add a Potential Incident(Suppose norwegian)</t>
+  </si>
+  <si>
+    <t>Click on the edit button of Potential Incident.</t>
+  </si>
+  <si>
+    <t>All the currently present work operation under the selected work type should be listed under work operation drop down.</t>
+  </si>
+  <si>
+    <t>Select a work operation</t>
+  </si>
+  <si>
+    <t>Create the potential incident  with name "Test"(can be any name of your choice) under the selected WT and WO</t>
+  </si>
+  <si>
+    <t>The Created potential incident should be added in the potential incident list with a success message under the selected wt and wo.</t>
+  </si>
+  <si>
+    <t>Again create a potential incident with name "test" under the same work type and work operation</t>
+  </si>
+  <si>
+    <t>The potential incident should not be created and the message "Duplicate potential incident should be displayed.</t>
+  </si>
+  <si>
+    <t>DBA_Settings_AddDuplicateConsequenceType</t>
+  </si>
+  <si>
+    <t>Verify that Consequence Type with the same name cannot be added</t>
+  </si>
+  <si>
+    <t>Click on the Edit button of Consequence Type</t>
+  </si>
+  <si>
+    <t>A popup module should appear with Add Consequence Type form and list.</t>
+  </si>
+  <si>
+    <t>Create the Consequence Type with name "Test"(can be any name of your choice)</t>
+  </si>
+  <si>
+    <t>The Created Consequence Type should be added in the Consequence Type list with a success message.</t>
+  </si>
+  <si>
+    <t>Again create a Consequence Type with name "test".</t>
+  </si>
+  <si>
+    <t>The Consequence Type should not be created and the message "Duplicate Work Type" should be displayed.</t>
+  </si>
+  <si>
+    <t>The name of the conequence type  should be unique.</t>
   </si>
 </sst>
 </file>
@@ -830,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,10 +1106,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>24</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -973,10 +1117,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -984,10 +1128,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
@@ -996,10 +1140,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1007,10 +1151,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1018,10 +1162,10 @@
         <v>2</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1029,10 +1173,10 @@
         <v>3</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1040,10 +1184,10 @@
         <v>4</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1051,10 +1195,10 @@
         <v>5</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1062,10 +1206,10 @@
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1073,10 +1217,10 @@
         <v>7</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1084,10 +1228,10 @@
         <v>8</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1095,10 +1239,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -1107,10 +1251,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1118,10 +1262,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1129,10 +1273,10 @@
         <v>2</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1140,10 +1284,10 @@
         <v>3</v>
       </c>
       <c r="F25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1151,22 +1295,22 @@
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1174,10 +1318,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1185,10 +1329,10 @@
         <v>2</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1196,10 +1340,10 @@
         <v>3</v>
       </c>
       <c r="F30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1207,10 +1351,10 @@
         <v>4</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1218,10 +1362,10 @@
         <v>5</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>10</v>
@@ -1230,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1241,10 +1385,10 @@
         <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1252,10 +1396,10 @@
         <v>2</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1263,10 +1407,10 @@
         <v>3</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1274,10 +1418,10 @@
         <v>4</v>
       </c>
       <c r="F37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1285,10 +1429,10 @@
         <v>6</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>10</v>
@@ -1297,10 +1441,10 @@
         <v>0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1308,10 +1452,10 @@
         <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1319,10 +1463,10 @@
         <v>2</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1330,10 +1474,10 @@
         <v>3</v>
       </c>
       <c r="F42" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1341,10 +1485,10 @@
         <v>4</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1352,10 +1496,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>10</v>
@@ -1364,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1375,10 +1519,10 @@
         <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1386,10 +1530,10 @@
         <v>2</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1397,10 +1541,10 @@
         <v>3</v>
       </c>
       <c r="F48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1408,10 +1552,10 @@
         <v>4</v>
       </c>
       <c r="F49" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1419,10 +1563,10 @@
         <v>5</v>
       </c>
       <c r="F50" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1430,10 +1574,10 @@
         <v>8</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>10</v>
@@ -1442,10 +1586,10 @@
         <v>0</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1453,10 +1597,10 @@
         <v>1</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1464,10 +1608,10 @@
         <v>2</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1475,10 +1619,10 @@
         <v>3</v>
       </c>
       <c r="F55" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1486,10 +1630,10 @@
         <v>4</v>
       </c>
       <c r="F56" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1497,10 +1641,10 @@
         <v>5</v>
       </c>
       <c r="F57" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G57" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1508,10 +1652,10 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>10</v>
@@ -1520,10 +1664,10 @@
         <v>0</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1531,10 +1675,10 @@
         <v>1</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1542,10 +1686,10 @@
         <v>2</v>
       </c>
       <c r="F61" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1553,10 +1697,10 @@
         <v>3</v>
       </c>
       <c r="F62" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1564,10 +1708,10 @@
         <v>4</v>
       </c>
       <c r="F63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1575,10 +1719,10 @@
         <v>10</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>10</v>
@@ -1587,10 +1731,10 @@
         <v>0</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1598,10 +1742,10 @@
         <v>1</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1609,10 +1753,10 @@
         <v>2</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1620,10 +1764,10 @@
         <v>3</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1631,10 +1775,10 @@
         <v>4</v>
       </c>
       <c r="F69" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1642,10 +1786,10 @@
         <v>5</v>
       </c>
       <c r="F70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G70" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1653,10 +1797,10 @@
         <v>11</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>10</v>
@@ -1665,10 +1809,10 @@
         <v>0</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1676,10 +1820,10 @@
         <v>1</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1687,10 +1831,10 @@
         <v>2</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1698,10 +1842,10 @@
         <v>3</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1709,10 +1853,10 @@
         <v>4</v>
       </c>
       <c r="F76" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G76" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1720,10 +1864,10 @@
         <v>5</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1731,10 +1875,10 @@
         <v>12</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>10</v>
@@ -1743,10 +1887,10 @@
         <v>0</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1754,10 +1898,10 @@
         <v>1</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1765,10 +1909,10 @@
         <v>2</v>
       </c>
       <c r="F81" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1776,10 +1920,10 @@
         <v>4</v>
       </c>
       <c r="F82" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G82" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1787,10 +1931,10 @@
         <v>13</v>
       </c>
       <c r="B84" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>10</v>
@@ -1799,10 +1943,10 @@
         <v>0</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1810,10 +1954,10 @@
         <v>1</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1821,10 +1965,10 @@
         <v>2</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1832,10 +1976,10 @@
         <v>3</v>
       </c>
       <c r="F87" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G87" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1843,10 +1987,10 @@
         <v>4</v>
       </c>
       <c r="F88" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G88" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1854,10 +1998,10 @@
         <v>14</v>
       </c>
       <c r="B90" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>10</v>
@@ -1866,10 +2010,10 @@
         <v>0</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1877,10 +2021,10 @@
         <v>1</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1888,10 +2032,10 @@
         <v>2</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1899,10 +2043,10 @@
         <v>3</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1910,18 +2054,384 @@
         <v>4</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>15</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="4">
+        <v>0</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="E97" s="4">
+        <v>1</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="E98" s="4">
+        <v>2</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E99" s="4">
+        <v>3</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E100" s="4">
+        <v>4</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E101" s="4">
+        <v>5</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>16</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" s="4">
+        <v>0</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E104" s="4">
+        <v>1</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E105" s="4">
+        <v>2</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E106" s="4">
+        <v>3</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E107" s="4">
+        <v>4</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>17</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E109" s="4">
+        <v>0</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E110" s="4">
+        <v>1</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E111" s="4">
+        <v>2</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E112" s="4">
+        <v>3</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E113" s="4">
+        <v>4</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E114" s="4">
+        <v>5</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G114" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <v>18</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" s="4">
+        <v>0</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E117" s="4">
+        <v>1</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E118" s="4">
+        <v>2</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E119" s="4">
+        <v>3</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E120" s="4">
+        <v>4</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="E121" s="4">
+        <v>4</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E122" s="4">
+        <v>5</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G122" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A124" s="6">
+        <v>19</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E124" s="4">
+        <v>0</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="6"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="6">
+        <v>1</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A126" s="6"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="6">
+        <v>2</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A127" s="6"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="6">
+        <v>3</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1934,7 +2444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1985,10 +2495,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -1997,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>

</xml_diff>